<commit_message>
summary as excel sheet
</commit_message>
<xml_diff>
--- a/Zusammenfassung.xlsx
+++ b/Zusammenfassung.xlsx
@@ -67,7 +67,7 @@
     <t>Datei</t>
   </si>
   <si>
-    <t>Auswertung_Susanne.xlsx</t>
+    <t>test.xlsx</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>44598.71816315263</v>
+        <v>44598.73328399118</v>
       </c>
     </row>
     <row r="9" spans="1:10">

</xml_diff>